<commit_message>
Set UI and fix some bugs
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stevenjoeng/Desktop/python-workspace/gojan-payslip-converter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\PycharmProjects\neis-to-payslip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3987CDEF-D5D2-3C45-A998-A47E7E3FDD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA8201-13F3-45BB-A1D0-E38AC0296554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="1240" windowWidth="26440" windowHeight="15440" xr2:uid="{63E6716E-172E-F54E-90CA-435E3BF7C4D2}"/>
+    <workbookView xWindow="5424" yWindow="1416" windowWidth="23040" windowHeight="12204" xr2:uid="{63E6716E-172E-F54E-90CA-435E3BF7C4D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>개인
 정보</t>
@@ -147,6 +147,14 @@
   <si>
     <t>1990.1.1.~
 정년</t>
+  </si>
+  <si>
+    <t>key=form</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>밑을 지우지 말아주세요!</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -154,15 +162,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="0.0_ "/>
-    <numFmt numFmtId="165" formatCode="0_ "/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -170,7 +178,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -186,7 +194,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -213,6 +221,13 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -547,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
@@ -573,40 +588,94 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -621,69 +690,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -699,7 +717,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -995,43 +1013,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBFF2862-C27B-FD4A-B976-07CC2A4E01E9}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" customWidth="1"/>
+    <col min="7" max="7" width="26.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" customHeight="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" ht="17" customHeight="1" thickBot="1">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-    </row>
-    <row r="3" spans="1:7" ht="17">
-      <c r="A3" s="37" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="43" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1053,8 +1071,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="36">
-      <c r="A4" s="38"/>
+    <row r="4" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.45">
+      <c r="A4" s="44"/>
       <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
@@ -1074,8 +1092,8 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18">
-      <c r="A5" s="39" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="33" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1084,10 +1102,10 @@
       <c r="C5" s="10">
         <v>31</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="42">
+      <c r="E5" s="36">
         <v>209</v>
       </c>
       <c r="F5" s="11" t="s">
@@ -1097,16 +1115,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="17">
-      <c r="A6" s="39"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="33"/>
       <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="14">
         <v>0</v>
       </c>
-      <c r="D6" s="41"/>
-      <c r="E6" s="43"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="37"/>
       <c r="F6" s="15">
         <v>0</v>
       </c>
@@ -1114,186 +1132,204 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18">
-      <c r="A7" s="39"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="33"/>
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="10">
         <v>0</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="17">
         <v>0</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18">
-      <c r="A8" s="39"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="33"/>
       <c r="B8" s="18" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="14">
         <v>0</v>
       </c>
-      <c r="D8" s="41"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="19">
         <v>0</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="1:7" ht="17">
-      <c r="A9" s="39"/>
-      <c r="B9" s="28" t="s">
+      <c r="F8" s="38"/>
+      <c r="G8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="33"/>
+      <c r="B9" s="24" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="10">
         <v>0</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="28">
         <v>20</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="F9" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="31">
         <f>ROUNDUP(((3000000+140000+39000*E9)/E5),2)</f>
         <v>18755.989999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="18" thickBot="1">
-      <c r="A10" s="40"/>
-      <c r="B10" s="29"/>
+    <row r="10" spans="1:7" ht="19.8" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="34"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="20">
         <v>0</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="36"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="22" t="s">
+      <c r="D10" s="27"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="32"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="22" t="s">
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="22" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="21" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-    </row>
-    <row r="16" spans="1:7" ht="16" customHeight="1">
-      <c r="A16" s="25" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+    </row>
+    <row r="16" spans="1:7" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="25"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B23" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="45"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B24" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="45"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="20">
+    <mergeCell ref="A1:G2"/>
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="A16:G22"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="B9:B10"/>
@@ -1308,11 +1344,8 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A1:G2"/>
-    <mergeCell ref="A14:G14"/>
-    <mergeCell ref="A12:G12"/>
-    <mergeCell ref="A3:A4"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>